<commit_message>
Carat: Update ShortByTeachers report
</commit_message>
<xml_diff>
--- a/Carat/templates/ShortByTeachers.xlsx
+++ b/Carat/templates/ShortByTeachers.xlsx
@@ -15,14 +15,14 @@
     <sheet name="Навантаження кафедри" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Навантаження кафедри'!$8:$9</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">'Навантаження кафедри'!$8:$8</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -30,73 +30,50 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ТЕФ</t>
-  </si>
-  <si>
     <t>(повна назва кафедри)</t>
   </si>
   <si>
-    <t>П.І.Б. викладача,
-посада, частка ставки</t>
-  </si>
-  <si>
-    <t>№ п/п</t>
-  </si>
-  <si>
-    <t>Інші аудиторні</t>
-  </si>
-  <si>
-    <t>Інші аудиторні</t>
-  </si>
-  <si>
-    <t>ВСЬОГО годин</t>
-  </si>
-  <si>
-    <t>Разом:</t>
-  </si>
-  <si>
-    <t>Разом:</t>
-  </si>
-  <si>
     <t>Кафедра автоматизації теплоенергетичних процесів</t>
   </si>
   <si>
     <t>Всього по кафедрі:</t>
   </si>
   <si>
-    <t xml:space="preserve">Факультет </t>
-  </si>
-  <si>
-    <t>Неаудиторні</t>
-  </si>
-  <si>
-    <t>Неаудиторні</t>
-  </si>
-  <si>
-    <t>Лекції</t>
-  </si>
-  <si>
-    <t>Лекції</t>
-  </si>
-  <si>
     <t>Навантаження кафедри за викладачами (спрощений)</t>
   </si>
   <si>
-    <t>II семестр, бюджет</t>
-  </si>
-  <si>
-    <t>Денна форма навчання</t>
-  </si>
-  <si>
-    <t>Заочна та вечірня
-форма навчання</t>
+    <t>За два семестри, бюджет</t>
+  </si>
+  <si>
+    <t>№ з/п</t>
+  </si>
+  <si>
+    <t>ПІБ викладача</t>
+  </si>
+  <si>
+    <t>Посада</t>
+  </si>
+  <si>
+    <t>Частка ставки</t>
+  </si>
+  <si>
+    <t>ВСЬОГО</t>
+  </si>
+  <si>
+    <t>Лекції, год.</t>
+  </si>
+  <si>
+    <t>Інші аудиторні, год.</t>
+  </si>
+  <si>
+    <t>Неаудиторні, год.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -139,29 +116,8 @@
       <charset val="204"/>
     </font>
     <font>
-      <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial Cyr"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial Cyr"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <b/>
       <sz val="8"/>
-      <color indexed="8"/>
-      <name val="Arial Cyr"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial Cyr"/>
       <charset val="204"/>
@@ -175,7 +131,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -211,15 +167,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -265,12 +212,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -283,72 +226,44 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" textRotation="90"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -633,232 +548,149 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" customWidth="1"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="11" width="6.7109375" customWidth="1"/>
+    <col min="3" max="3" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="11"/>
-      <c r="I2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="9"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="26"/>
-      <c r="D5" s="26"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="26"/>
-      <c r="G5" s="26"/>
-      <c r="H5" s="26"/>
-      <c r="I5" s="26"/>
-      <c r="J5" s="26"/>
-      <c r="K5" s="26"/>
-    </row>
-    <row r="6" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B4" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+    </row>
+    <row r="6" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="26.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="27" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="29" t="s">
+    <row r="8" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+    </row>
+    <row r="10" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+      <c r="C10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="28"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="I9" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="K9" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="L9" s="24"/>
-    </row>
-    <row r="10" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-    </row>
-    <row r="11" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="3"/>
-      <c r="C11" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="20">
-        <f>SUM(D10:D10)</f>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="13">
+        <f>SUM(F9:F9)</f>
         <v>0</v>
       </c>
-      <c r="E11" s="20">
-        <f>SUM(E10:E10)</f>
+      <c r="G10" s="13">
+        <f>SUM(G9:G9)</f>
         <v>0</v>
       </c>
-      <c r="F11" s="20">
-        <f>SUM(F10:F10)</f>
+      <c r="H10" s="13">
+        <f>SUM(H9:H9)</f>
         <v>0</v>
       </c>
-      <c r="G11" s="19">
-        <f t="shared" ref="G11" si="0">SUM(D11:F11)</f>
+      <c r="I10" s="13">
+        <f>SUM(I9:I9)</f>
         <v>0</v>
       </c>
-      <c r="H11" s="20">
-        <f>SUM(H10:H10)</f>
-        <v>0</v>
-      </c>
-      <c r="I11" s="20">
-        <f>SUM(I10:I10)</f>
-        <v>0</v>
-      </c>
-      <c r="J11" s="20">
-        <f>SUM(J10:J10)</f>
-        <v>0</v>
-      </c>
-      <c r="K11" s="19">
-        <f t="shared" ref="K11" si="1">SUM(H11:J11)</f>
-        <v>0</v>
-      </c>
-      <c r="L11" s="19">
-        <f t="shared" ref="L11" si="2">G11+K11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H12" s="2"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="31" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="D8:G8"/>
-    <mergeCell ref="H8:K8"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="B5:K5"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:C9"/>
+  <mergeCells count="2">
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="B5:H5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0" footer="0"/>
+  <pageMargins left="0.196850393700787" right="0.196850393700787" top="0.196850393700787" bottom="0.196850393700787" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>

</xml_diff>

<commit_message>
Carat: Fix of bugs
</commit_message>
<xml_diff>
--- a/Carat/templates/ShortByTeachers.xlsx
+++ b/Carat/templates/ShortByTeachers.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Неаудиторні, год.</t>
+  </si>
+  <si>
+    <t>Форма зайнятості</t>
   </si>
 </sst>
 </file>
@@ -212,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -259,16 +262,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -554,10 +566,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E10"/>
+      <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -570,18 +582,18 @@
     <col min="6" max="8" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="6"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>2</v>
       </c>
@@ -592,29 +604,29 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B4" s="16" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B4" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="17" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
+      <c r="H4" s="18"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="17"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-    </row>
-    <row r="6" spans="1:9" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:10" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -623,12 +635,12 @@
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
         <v>7</v>
       </c>
@@ -641,42 +653,43 @@
       <c r="E8" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="H8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="J8" s="12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>1</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="9"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="21"/>
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9"/>
-    </row>
-    <row r="10" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1"/>
       <c r="C10" s="8" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="19"/>
-      <c r="F10" s="13">
-        <f>SUM(F9:F9)</f>
-        <v>0</v>
-      </c>
+      <c r="E10" s="17"/>
+      <c r="F10" s="22"/>
       <c r="G10" s="13">
         <f>SUM(G9:G9)</f>
         <v>0</v>
@@ -687,6 +700,10 @@
       </c>
       <c r="I10" s="13">
         <f>SUM(I9:I9)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="13">
+        <f>SUM(J9:J9)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>